<commit_message>
Added a mechanism to prevent the database from recieving and duplicate entries in monthly or weekly data
</commit_message>
<xml_diff>
--- a/reports/monthly/MARCH_monthly_report.xlsx
+++ b/reports/monthly/MARCH_monthly_report.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/63f515c073db2062/Desktop/Data Science w Cloiud/Meta Ad Analysis Project/Ad-Data-Analysis-Lingerie/reports/monthly/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="11_351134B7A087A001485B80B4F5953C256BCCB689" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BA3EB128-A6EF-4F2E-A1D9-F0661A116087}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="48">
   <si>
     <t>campaign_name</t>
   </si>
@@ -169,8 +163,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -195,31 +189,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -249,36 +225,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -316,7 +281,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -350,7 +315,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -385,10 +349,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -561,30 +524,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AD20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="39.88671875" customWidth="1"/>
-    <col min="2" max="2" width="38.77734375" customWidth="1"/>
-    <col min="3" max="3" width="56.21875" customWidth="1"/>
-    <col min="4" max="4" width="18.44140625" customWidth="1"/>
-    <col min="5" max="5" width="20.77734375" customWidth="1"/>
-    <col min="6" max="6" width="17.77734375" customWidth="1"/>
-    <col min="7" max="7" width="22" customWidth="1"/>
-    <col min="8" max="8" width="20.44140625" customWidth="1"/>
-    <col min="9" max="9" width="35" customWidth="1"/>
-    <col min="10" max="10" width="34" customWidth="1"/>
-    <col min="11" max="11" width="27.109375" customWidth="1"/>
-    <col min="12" max="12" width="36.6640625" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30">
       <c r="A1" s="1" t="s">
         <v>45</v>
       </c>
@@ -676,104 +623,104 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" s="5">
-        <v>864.51999998999997</v>
-      </c>
-      <c r="C2" s="5">
+    <row r="2" spans="1:30">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2">
+        <v>864.51999999</v>
+      </c>
+      <c r="C2">
         <v>47</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2">
         <v>94769</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2">
         <v>384</v>
       </c>
-      <c r="F2" s="5">
-        <v>18.394042552978721</v>
-      </c>
-      <c r="G2" s="5">
-        <v>9.1223923433823302</v>
-      </c>
-      <c r="H2" s="5">
-        <v>2.2513541666406249</v>
-      </c>
-      <c r="I2" s="5">
-        <v>817.02127659574467</v>
-      </c>
-      <c r="J2" s="5">
-        <v>779.97999999000001</v>
-      </c>
-      <c r="K2" s="5">
+      <c r="F2">
+        <v>18.39404255297872</v>
+      </c>
+      <c r="G2">
+        <v>9.12239234338233</v>
+      </c>
+      <c r="H2">
+        <v>2.251354166640625</v>
+      </c>
+      <c r="I2">
+        <v>817.0212765957447</v>
+      </c>
+      <c r="J2">
+        <v>779.97999999</v>
+      </c>
+      <c r="K2">
         <v>62</v>
       </c>
-      <c r="L2" s="5">
+      <c r="L2">
         <v>76113</v>
       </c>
-      <c r="M2" s="5">
+      <c r="M2">
         <v>339</v>
       </c>
-      <c r="N2" s="5">
+      <c r="N2">
         <v>12.58032258048387</v>
       </c>
-      <c r="O2" s="5">
+      <c r="O2">
         <v>10.24765808718616</v>
       </c>
-      <c r="P2" s="5">
-        <v>2.3008259586725659</v>
-      </c>
-      <c r="Q2" s="5">
-        <v>546.77419354838707</v>
-      </c>
-      <c r="R2" s="5">
-        <v>10.838739454996769</v>
-      </c>
-      <c r="S2" s="5">
-        <v>-24.193548387096779</v>
-      </c>
-      <c r="T2" s="5">
-        <v>46.212805238506363</v>
-      </c>
-      <c r="U2" s="5">
-        <v>24.510924546398119</v>
-      </c>
-      <c r="V2" s="5">
+      <c r="P2">
+        <v>2.300825958672566</v>
+      </c>
+      <c r="Q2">
+        <v>546.7741935483871</v>
+      </c>
+      <c r="R2">
+        <v>10.83873945499677</v>
+      </c>
+      <c r="S2">
+        <v>-24.19354838709678</v>
+      </c>
+      <c r="T2">
+        <v>46.21280523850636</v>
+      </c>
+      <c r="U2">
+        <v>24.51092454639812</v>
+      </c>
+      <c r="V2">
         <v>-10.98071124378046</v>
       </c>
-      <c r="W2" s="5">
-        <v>13.274336283185839</v>
-      </c>
-      <c r="X2" s="5">
-        <v>-2.1501753248856579</v>
-      </c>
-      <c r="Y2" s="5">
-        <v>49.425720203351538</v>
-      </c>
-      <c r="Z2" s="5">
+      <c r="W2">
+        <v>13.27433628318584</v>
+      </c>
+      <c r="X2">
+        <v>-2.150175324885658</v>
+      </c>
+      <c r="Y2">
+        <v>49.42572020335154</v>
+      </c>
+      <c r="Z2">
         <v>141.8699054776759</v>
       </c>
-      <c r="AA2" s="5">
+      <c r="AA2">
         <v>-12.61455692392432</v>
       </c>
-      <c r="AB2" s="5">
-        <v>38.014034060376517</v>
-      </c>
-      <c r="AC2" s="5">
+      <c r="AB2">
+        <v>38.01403406037652</v>
+      </c>
+      <c r="AC2">
         <v>118.0456970566229</v>
       </c>
-      <c r="AD2" s="5" t="s">
+      <c r="AD2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:30">
       <c r="A3" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:30">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -808,82 +755,82 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5" s="5" t="s">
+    <row r="5" spans="1:30">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5">
         <v>509.73999999</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5">
         <v>34</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5">
         <v>54121</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5">
         <v>193</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5">
         <v>14.99235294088235</v>
       </c>
-      <c r="H5" s="5">
-        <v>9.4185251564087871</v>
-      </c>
-      <c r="I5" s="5">
-        <v>2.6411398963212429</v>
-      </c>
-      <c r="J5" s="5">
-        <v>567.64705882352939</v>
-      </c>
-      <c r="K5" s="5" t="s">
+      <c r="H5">
+        <v>9.418525156408787</v>
+      </c>
+      <c r="I5">
+        <v>2.641139896321243</v>
+      </c>
+      <c r="J5">
+        <v>567.6470588235294</v>
+      </c>
+      <c r="K5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="5" t="s">
+    <row r="6" spans="1:30">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6">
         <v>354.78</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6">
         <v>13</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6">
         <v>40648</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6">
         <v>191</v>
       </c>
-      <c r="G6" s="5">
-        <v>27.290769230769229</v>
-      </c>
-      <c r="H6" s="5">
-        <v>8.7281047037984667</v>
-      </c>
-      <c r="I6" s="5">
+      <c r="G6">
+        <v>27.29076923076923</v>
+      </c>
+      <c r="H6">
+        <v>8.728104703798467</v>
+      </c>
+      <c r="I6">
         <v>1.857486910994764</v>
       </c>
-      <c r="J6" s="5">
-        <v>1469.2307692307691</v>
-      </c>
-      <c r="K6" s="5" t="s">
+      <c r="J6">
+        <v>1469.230769230769</v>
+      </c>
+      <c r="K6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:30">
       <c r="A7" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:30">
       <c r="A8" s="2" t="s">
         <v>0</v>
       </c>
@@ -921,420 +868,420 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" s="3" t="s">
+    <row r="9" spans="1:30">
+      <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9">
         <v>32.89</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9">
         <v>0</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9">
         <v>3656</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9">
         <v>16</v>
       </c>
-      <c r="I9" s="3">
-        <v>8.9961706783369806</v>
-      </c>
-      <c r="J9" s="3">
+      <c r="I9">
+        <v>8.996170678336981</v>
+      </c>
+      <c r="J9">
         <v>2.055625</v>
       </c>
-      <c r="L9" s="3" t="s">
+      <c r="L9" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="5" t="s">
+    <row r="10" spans="1:30">
+      <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10">
         <v>114.39</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10">
         <v>9</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10">
         <v>13676</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10">
         <v>60</v>
       </c>
-      <c r="H10" s="5">
+      <c r="H10">
         <v>12.71</v>
       </c>
-      <c r="I10" s="5">
-        <v>8.3642878034513011</v>
-      </c>
-      <c r="J10" s="5">
-        <v>1.9065000000000001</v>
-      </c>
-      <c r="K10" s="5">
-        <v>666.66666666666674</v>
-      </c>
-      <c r="L10" s="5" t="s">
+      <c r="I10">
+        <v>8.364287803451301</v>
+      </c>
+      <c r="J10">
+        <v>1.9065</v>
+      </c>
+      <c r="K10">
+        <v>666.6666666666667</v>
+      </c>
+      <c r="L10" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="4" t="s">
+    <row r="11" spans="1:30">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11">
         <v>3.36</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11">
         <v>0</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11">
         <v>376</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11">
         <v>4</v>
       </c>
-      <c r="I11" s="4">
-        <v>8.9361702127659584</v>
-      </c>
-      <c r="J11" s="4">
+      <c r="I11">
+        <v>8.936170212765958</v>
+      </c>
+      <c r="J11">
         <v>0.84</v>
       </c>
-      <c r="L11" s="4" t="s">
+      <c r="L11" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="4" t="s">
+    <row r="12" spans="1:30">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12">
         <v>10.66</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12">
         <v>0</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12">
         <v>1217</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12">
         <v>4</v>
       </c>
-      <c r="I12" s="4">
-        <v>8.7592440427280209</v>
-      </c>
-      <c r="J12" s="4">
+      <c r="I12">
+        <v>8.759244042728021</v>
+      </c>
+      <c r="J12">
         <v>2.665</v>
       </c>
-      <c r="L12" s="4" t="s">
+      <c r="L12" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="4" t="s">
+    <row r="13" spans="1:30">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="4">
-        <v>17.739999999999998</v>
-      </c>
-      <c r="E13" s="4">
+      <c r="D13">
+        <v>17.74</v>
+      </c>
+      <c r="E13">
         <v>0</v>
       </c>
-      <c r="F13" s="4">
+      <c r="F13">
         <v>1972</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G13">
         <v>17</v>
       </c>
-      <c r="I13" s="4">
-        <v>8.9959432048681531</v>
-      </c>
-      <c r="J13" s="4">
+      <c r="I13">
+        <v>8.995943204868153</v>
+      </c>
+      <c r="J13">
         <v>1.043529411764706</v>
       </c>
-      <c r="L13" s="4" t="s">
+      <c r="L13" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" s="5" t="s">
+    <row r="14" spans="1:30">
+      <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14">
         <v>87.94</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14">
         <v>8</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14">
         <v>6002</v>
       </c>
-      <c r="G14" s="5">
+      <c r="G14">
         <v>32</v>
       </c>
-      <c r="H14" s="5">
+      <c r="H14">
         <v>10.9925</v>
       </c>
-      <c r="I14" s="5">
+      <c r="I14">
         <v>14.65178273908697</v>
       </c>
-      <c r="J14" s="5">
-        <v>2.7481249999999999</v>
-      </c>
-      <c r="K14" s="5">
+      <c r="J14">
+        <v>2.748125</v>
+      </c>
+      <c r="K14">
         <v>400</v>
       </c>
-      <c r="L14" s="5" t="s">
+      <c r="L14" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="4" t="s">
+    <row r="15" spans="1:30">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15">
         <v>0.46</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15">
         <v>0</v>
       </c>
-      <c r="F15" s="4">
+      <c r="F15">
         <v>46</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G15">
         <v>0</v>
       </c>
-      <c r="I15" s="4">
+      <c r="I15">
         <v>10</v>
       </c>
-      <c r="L15" s="4" t="s">
+      <c r="L15" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="4" t="s">
+    <row r="16" spans="1:30">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="4">
-        <v>30</v>
-      </c>
-      <c r="E16" s="4">
+      <c r="D16">
+        <v>30</v>
+      </c>
+      <c r="E16">
         <v>0</v>
       </c>
-      <c r="F16" s="4">
+      <c r="F16">
         <v>3260</v>
       </c>
-      <c r="G16" s="4">
+      <c r="G16">
         <v>10</v>
       </c>
-      <c r="I16" s="4">
-        <v>9.2024539877300615</v>
-      </c>
-      <c r="J16" s="4">
+      <c r="I16">
+        <v>9.202453987730062</v>
+      </c>
+      <c r="J16">
         <v>3</v>
       </c>
-      <c r="L16" s="4" t="s">
+      <c r="L16" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="5" t="s">
+    <row r="17" spans="1:12">
+      <c r="A17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17">
         <v>102.6</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17">
         <v>2</v>
       </c>
-      <c r="F17" s="5">
+      <c r="F17">
         <v>13131</v>
       </c>
-      <c r="G17" s="5">
+      <c r="G17">
         <v>34</v>
       </c>
-      <c r="H17" s="5">
+      <c r="H17">
         <v>51.3</v>
       </c>
-      <c r="I17" s="5">
-        <v>7.8135709389993142</v>
-      </c>
-      <c r="J17" s="5">
-        <v>3.0176470588235298</v>
-      </c>
-      <c r="K17" s="5">
+      <c r="I17">
+        <v>7.813570938999314</v>
+      </c>
+      <c r="J17">
+        <v>3.01764705882353</v>
+      </c>
+      <c r="K17">
         <v>1700</v>
       </c>
-      <c r="L17" s="5" t="s">
+      <c r="L17" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" s="5" t="s">
+    <row r="18" spans="1:12">
+      <c r="A18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="5">
-        <v>348.24999998999999</v>
-      </c>
-      <c r="E18" s="5">
+      <c r="D18">
+        <v>348.24999999</v>
+      </c>
+      <c r="E18">
         <v>26</v>
       </c>
-      <c r="F18" s="5">
+      <c r="F18">
         <v>39986</v>
       </c>
-      <c r="G18" s="5">
+      <c r="G18">
         <v>131</v>
       </c>
-      <c r="H18" s="5">
+      <c r="H18">
         <v>13.39423076884616</v>
       </c>
-      <c r="I18" s="5">
-        <v>8.7092982541389503</v>
-      </c>
-      <c r="J18" s="5">
+      <c r="I18">
+        <v>8.70929825413895</v>
+      </c>
+      <c r="J18">
         <v>2.65839694648855</v>
       </c>
-      <c r="K18" s="5">
-        <v>503.84615384615381</v>
-      </c>
-      <c r="L18" s="5" t="s">
+      <c r="K18">
+        <v>503.8461538461538</v>
+      </c>
+      <c r="L18" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" s="5" t="s">
+    <row r="19" spans="1:12">
+      <c r="A19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" t="s">
         <v>34</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D19">
         <v>48.55</v>
       </c>
-      <c r="E19" s="5">
+      <c r="E19">
         <v>1</v>
       </c>
-      <c r="F19" s="5">
+      <c r="F19">
         <v>6195</v>
       </c>
-      <c r="G19" s="5">
-        <v>30</v>
-      </c>
-      <c r="H19" s="5">
+      <c r="G19">
+        <v>30</v>
+      </c>
+      <c r="H19">
         <v>48.55</v>
       </c>
-      <c r="I19" s="5">
-        <v>7.8369652945924146</v>
-      </c>
-      <c r="J19" s="5">
+      <c r="I19">
+        <v>7.836965294592415</v>
+      </c>
+      <c r="J19">
         <v>1.618333333333333</v>
       </c>
-      <c r="K19" s="5">
+      <c r="K19">
         <v>3000</v>
       </c>
-      <c r="L19" s="5" t="s">
+      <c r="L19" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B20" s="5" t="s">
+    <row r="20" spans="1:12">
+      <c r="A20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" t="s">
         <v>34</v>
       </c>
-      <c r="D20" s="5">
-        <v>67.680000000000007</v>
-      </c>
-      <c r="E20" s="5">
+      <c r="D20">
+        <v>67.68000000000001</v>
+      </c>
+      <c r="E20">
         <v>1</v>
       </c>
-      <c r="F20" s="5">
+      <c r="F20">
         <v>5252</v>
       </c>
-      <c r="G20" s="5">
+      <c r="G20">
         <v>46</v>
       </c>
-      <c r="H20" s="5">
-        <v>67.680000000000007</v>
-      </c>
-      <c r="I20" s="5">
+      <c r="H20">
+        <v>67.68000000000001</v>
+      </c>
+      <c r="I20">
         <v>12.88651942117289</v>
       </c>
-      <c r="J20" s="5">
+      <c r="J20">
         <v>1.471304347826087</v>
       </c>
-      <c r="K20" s="5">
+      <c r="K20">
         <v>4600</v>
       </c>
-      <c r="L20" s="5" t="s">
+      <c r="L20" t="s">
         <v>44</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Removed 0 results and improved csv formatting
</commit_message>
<xml_diff>
--- a/reports/monthly/MARCH_monthly_report.xlsx
+++ b/reports/monthly/MARCH_monthly_report.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="46">
   <si>
     <t>campaign_name</t>
   </si>
@@ -128,12 +128,6 @@
   </si>
   <si>
     <t>elec|ifd-stor-rl|img|purple_cta_bulb</t>
-  </si>
-  <si>
-    <t>gen|ifd-stor-rl|img|cta_purple_bulb</t>
-  </si>
-  <si>
-    <t>gen|ifd-stor-rl|img|greentextonly</t>
   </si>
   <si>
     <t>gen|ifd-stor-rl|vid|introvideo</t>
@@ -525,7 +519,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AD20"/>
+  <dimension ref="A1:AD14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -533,7 +527,7 @@
   <sheetData>
     <row r="1" spans="1:30">
       <c r="A1" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -628,88 +622,88 @@
         <v>30</v>
       </c>
       <c r="B2">
-        <v>864.51999999</v>
+        <v>583.39287734</v>
       </c>
       <c r="C2">
         <v>47</v>
       </c>
       <c r="D2">
-        <v>94769</v>
+        <v>63609</v>
       </c>
       <c r="E2">
-        <v>384</v>
+        <v>230</v>
       </c>
       <c r="F2">
-        <v>18.39404255297872</v>
+        <v>12.41261441148936</v>
       </c>
       <c r="G2">
-        <v>9.12239234338233</v>
+        <v>9.171546123032904</v>
       </c>
       <c r="H2">
-        <v>2.251354166640625</v>
+        <v>2.536490771043479</v>
       </c>
       <c r="I2">
-        <v>817.0212765957447</v>
+        <v>489.3617021276596</v>
       </c>
       <c r="J2">
-        <v>779.97999999</v>
+        <v>584.89944804</v>
       </c>
       <c r="K2">
         <v>62</v>
       </c>
       <c r="L2">
-        <v>76113</v>
+        <v>56540</v>
       </c>
       <c r="M2">
-        <v>339</v>
+        <v>245</v>
       </c>
       <c r="N2">
-        <v>12.58032258048387</v>
+        <v>9.433862065161291</v>
       </c>
       <c r="O2">
-        <v>10.24765808718616</v>
+        <v>10.34487881216838</v>
       </c>
       <c r="P2">
-        <v>2.300825958672566</v>
+        <v>2.387344685877551</v>
       </c>
       <c r="Q2">
-        <v>546.7741935483871</v>
+        <v>395.1612903225807</v>
       </c>
       <c r="R2">
-        <v>10.83873945499677</v>
+        <v>-0.2575777264021228</v>
       </c>
       <c r="S2">
         <v>-24.19354838709678</v>
       </c>
       <c r="T2">
-        <v>46.21280523850636</v>
+        <v>31.57511023325678</v>
       </c>
       <c r="U2">
-        <v>24.51092454639812</v>
+        <v>12.50265298903431</v>
       </c>
       <c r="V2">
-        <v>-10.98071124378046</v>
+        <v>-11.34215983038213</v>
       </c>
       <c r="W2">
-        <v>13.27433628318584</v>
+        <v>-6.122448979591836</v>
       </c>
       <c r="X2">
-        <v>-2.150175324885658</v>
+        <v>6.247362856658605</v>
       </c>
       <c r="Y2">
-        <v>49.42572020335154</v>
+        <v>23.83847155883629</v>
       </c>
       <c r="Z2">
-        <v>141.8699054776759</v>
+        <v>106.7458255719991</v>
       </c>
       <c r="AA2">
-        <v>-12.61455692392432</v>
+        <v>-13.49332023745113</v>
       </c>
       <c r="AB2">
-        <v>38.01403406037652</v>
+        <v>53.61629419563344</v>
       </c>
       <c r="AC2">
-        <v>118.0456970566229</v>
+        <v>67.43044189852702</v>
       </c>
       <c r="AD2" t="s">
         <v>31</v>
@@ -717,7 +711,7 @@
     </row>
     <row r="3" spans="1:30">
       <c r="A3" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:30">
@@ -763,28 +757,28 @@
         <v>33</v>
       </c>
       <c r="C5">
-        <v>509.73999999</v>
+        <v>416.25744999</v>
       </c>
       <c r="D5">
         <v>34</v>
       </c>
       <c r="E5">
-        <v>54121</v>
+        <v>43611</v>
       </c>
       <c r="F5">
-        <v>193</v>
+        <v>151</v>
       </c>
       <c r="G5">
-        <v>14.99235294088235</v>
+        <v>12.24286617617647</v>
       </c>
       <c r="H5">
-        <v>9.418525156408787</v>
+        <v>9.544781132971039</v>
       </c>
       <c r="I5">
-        <v>2.641139896321243</v>
+        <v>2.756671854238411</v>
       </c>
       <c r="J5">
-        <v>567.6470588235294</v>
+        <v>444.1176470588235</v>
       </c>
       <c r="K5" t="s">
         <v>35</v>
@@ -798,28 +792,28 @@
         <v>34</v>
       </c>
       <c r="C6">
-        <v>354.78</v>
+        <v>167.13542735</v>
       </c>
       <c r="D6">
         <v>13</v>
       </c>
       <c r="E6">
-        <v>40648</v>
+        <v>19998</v>
       </c>
       <c r="F6">
-        <v>191</v>
+        <v>79</v>
       </c>
       <c r="G6">
-        <v>27.29076923076923</v>
+        <v>12.85657133461538</v>
       </c>
       <c r="H6">
-        <v>8.728104703798467</v>
+        <v>8.35760712821282</v>
       </c>
       <c r="I6">
-        <v>1.857486910994764</v>
+        <v>2.115638320886076</v>
       </c>
       <c r="J6">
-        <v>1469.230769230769</v>
+        <v>607.6923076923076</v>
       </c>
       <c r="K6" t="s">
         <v>35</v>
@@ -827,7 +821,7 @@
     </row>
     <row r="7" spans="1:30">
       <c r="A7" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:30">
@@ -876,28 +870,34 @@
         <v>37</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D9">
-        <v>32.89</v>
+        <v>98.19</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F9">
-        <v>3656</v>
+        <v>11671</v>
       </c>
       <c r="G9">
-        <v>16</v>
+        <v>46</v>
+      </c>
+      <c r="H9">
+        <v>10.91</v>
       </c>
       <c r="I9">
-        <v>8.996170678336981</v>
+        <v>8.413160825978922</v>
       </c>
       <c r="J9">
-        <v>2.055625</v>
+        <v>2.134565217391304</v>
+      </c>
+      <c r="K9">
+        <v>511.1111111111111</v>
       </c>
       <c r="L9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:30">
@@ -905,37 +905,37 @@
         <v>30</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D10">
-        <v>114.39</v>
+        <v>77.98773658</v>
       </c>
       <c r="E10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F10">
-        <v>13676</v>
+        <v>5245</v>
       </c>
       <c r="G10">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="H10">
-        <v>12.71</v>
+        <v>9.7484670725</v>
       </c>
       <c r="I10">
-        <v>8.364287803451301</v>
+        <v>14.86896788941849</v>
       </c>
       <c r="J10">
-        <v>1.9065</v>
+        <v>2.785276306428571</v>
       </c>
       <c r="K10">
-        <v>666.6666666666667</v>
+        <v>350</v>
       </c>
       <c r="L10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:30">
@@ -943,31 +943,37 @@
         <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C11" t="s">
         <v>34</v>
       </c>
       <c r="D11">
-        <v>3.36</v>
+        <v>46.91542735</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F11">
-        <v>376</v>
+        <v>5487</v>
       </c>
       <c r="G11">
-        <v>4</v>
+        <v>15</v>
+      </c>
+      <c r="H11">
+        <v>23.457713675</v>
       </c>
       <c r="I11">
-        <v>8.936170212765958</v>
+        <v>8.550287470384546</v>
       </c>
       <c r="J11">
-        <v>0.84</v>
+        <v>3.127695156666667</v>
+      </c>
+      <c r="K11">
+        <v>750</v>
       </c>
       <c r="L11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:30">
@@ -975,31 +981,37 @@
         <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C12" t="s">
         <v>33</v>
       </c>
       <c r="D12">
-        <v>10.66</v>
+        <v>338.26971341</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="F12">
-        <v>1217</v>
+        <v>38366</v>
       </c>
       <c r="G12">
-        <v>4</v>
+        <v>123</v>
+      </c>
+      <c r="H12">
+        <v>13.01037359269231</v>
       </c>
       <c r="I12">
-        <v>8.759244042728021</v>
+        <v>8.816913762445916</v>
       </c>
       <c r="J12">
-        <v>2.665</v>
+        <v>2.750160271626017</v>
+      </c>
+      <c r="K12">
+        <v>473.0769230769231</v>
       </c>
       <c r="L12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:30">
@@ -1007,31 +1019,37 @@
         <v>30</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C13" t="s">
         <v>34</v>
       </c>
       <c r="D13">
-        <v>17.74</v>
+        <v>19.05</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13">
-        <v>1972</v>
+        <v>2687</v>
       </c>
       <c r="G13">
         <v>17</v>
       </c>
+      <c r="H13">
+        <v>19.05</v>
+      </c>
       <c r="I13">
-        <v>8.995943204868153</v>
+        <v>7.089691105321921</v>
       </c>
       <c r="J13">
-        <v>1.043529411764706</v>
+        <v>1.120588235294118</v>
+      </c>
+      <c r="K13">
+        <v>1700</v>
       </c>
       <c r="L13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:30">
@@ -1039,250 +1057,37 @@
         <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C14" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D14">
-        <v>87.94</v>
+        <v>2.98</v>
       </c>
       <c r="E14">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F14">
-        <v>6002</v>
+        <v>153</v>
       </c>
       <c r="G14">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="H14">
-        <v>10.9925</v>
+        <v>2.98</v>
       </c>
       <c r="I14">
-        <v>14.65178273908697</v>
+        <v>19.47712418300653</v>
       </c>
       <c r="J14">
-        <v>2.748125</v>
+        <v>2.98</v>
       </c>
       <c r="K14">
-        <v>400</v>
+        <v>100</v>
       </c>
       <c r="L14" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:30">
-      <c r="A15" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15" t="s">
-        <v>34</v>
-      </c>
-      <c r="D15">
-        <v>0.46</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
-        <v>46</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="I15">
-        <v>10</v>
-      </c>
-      <c r="L15" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:30">
-      <c r="A16" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16" t="s">
-        <v>33</v>
-      </c>
-      <c r="D16">
-        <v>30</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <v>3260</v>
-      </c>
-      <c r="G16">
-        <v>10</v>
-      </c>
-      <c r="I16">
-        <v>9.202453987730062</v>
-      </c>
-      <c r="J16">
-        <v>3</v>
-      </c>
-      <c r="L16" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12">
-      <c r="A17" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" t="s">
-        <v>41</v>
-      </c>
-      <c r="C17" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17">
-        <v>102.6</v>
-      </c>
-      <c r="E17">
-        <v>2</v>
-      </c>
-      <c r="F17">
-        <v>13131</v>
-      </c>
-      <c r="G17">
-        <v>34</v>
-      </c>
-      <c r="H17">
-        <v>51.3</v>
-      </c>
-      <c r="I17">
-        <v>7.813570938999314</v>
-      </c>
-      <c r="J17">
-        <v>3.01764705882353</v>
-      </c>
-      <c r="K17">
-        <v>1700</v>
-      </c>
-      <c r="L17" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12">
-      <c r="A18" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" t="s">
         <v>42</v>
-      </c>
-      <c r="C18" t="s">
-        <v>33</v>
-      </c>
-      <c r="D18">
-        <v>348.24999999</v>
-      </c>
-      <c r="E18">
-        <v>26</v>
-      </c>
-      <c r="F18">
-        <v>39986</v>
-      </c>
-      <c r="G18">
-        <v>131</v>
-      </c>
-      <c r="H18">
-        <v>13.39423076884616</v>
-      </c>
-      <c r="I18">
-        <v>8.70929825413895</v>
-      </c>
-      <c r="J18">
-        <v>2.65839694648855</v>
-      </c>
-      <c r="K18">
-        <v>503.8461538461538</v>
-      </c>
-      <c r="L18" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12">
-      <c r="A19" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" t="s">
-        <v>42</v>
-      </c>
-      <c r="C19" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19">
-        <v>48.55</v>
-      </c>
-      <c r="E19">
-        <v>1</v>
-      </c>
-      <c r="F19">
-        <v>6195</v>
-      </c>
-      <c r="G19">
-        <v>30</v>
-      </c>
-      <c r="H19">
-        <v>48.55</v>
-      </c>
-      <c r="I19">
-        <v>7.836965294592415</v>
-      </c>
-      <c r="J19">
-        <v>1.618333333333333</v>
-      </c>
-      <c r="K19">
-        <v>3000</v>
-      </c>
-      <c r="L19" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12">
-      <c r="A20" t="s">
-        <v>30</v>
-      </c>
-      <c r="B20" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20" t="s">
-        <v>34</v>
-      </c>
-      <c r="D20">
-        <v>67.68000000000001</v>
-      </c>
-      <c r="E20">
-        <v>1</v>
-      </c>
-      <c r="F20">
-        <v>5252</v>
-      </c>
-      <c r="G20">
-        <v>46</v>
-      </c>
-      <c r="H20">
-        <v>67.68000000000001</v>
-      </c>
-      <c r="I20">
-        <v>12.88651942117289</v>
-      </c>
-      <c r="J20">
-        <v>1.471304347826087</v>
-      </c>
-      <c r="K20">
-        <v>4600</v>
-      </c>
-      <c r="L20" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>